<commit_message>
Escenarios casos de uso + correccion de id
</commit_message>
<xml_diff>
--- a/Documentacion/ECU/2- Ocupar mesa.xlsx
+++ b/Documentacion/ECU/2- Ocupar mesa.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucio\Desktop\Proyecto\SistemaRestaurante-master\Documentacion\ECU\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Escenario de Caso de Uso" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -78,9 +83,6 @@
     <t>Externa</t>
   </si>
   <si>
-    <t>Iniciar sesion</t>
-  </si>
-  <si>
     <t>Sistema Restaurante</t>
   </si>
   <si>
@@ -118,13 +120,16 @@
   </si>
   <si>
     <t>ID única: 002</t>
+  </si>
+  <si>
+    <t>Ocupar mesa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -543,21 +548,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+      <selection activeCell="B2" sqref="B2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.7109375" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" customWidth="1"/>
@@ -565,29 +570,29 @@
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.9" customHeight="1">
+    <row r="1" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D1" s="12"/>
     </row>
-    <row r="2" spans="1:4" ht="22.9" customHeight="1">
+    <row r="2" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
     </row>
-    <row r="3" spans="1:4" ht="22.9" customHeight="1">
+    <row r="3" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -597,27 +602,27 @@
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
     </row>
-    <row r="4" spans="1:4" ht="33" customHeight="1">
+    <row r="4" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:4" ht="22.9" customHeight="1">
+    <row r="5" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" spans="1:4" ht="22.9" customHeight="1">
+    <row r="6" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -627,7 +632,7 @@
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
     </row>
-    <row r="7" spans="1:4" ht="22.9" customHeight="1">
+    <row r="7" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -637,77 +642,77 @@
       <c r="C7" s="15"/>
       <c r="D7" s="16"/>
     </row>
-    <row r="8" spans="1:4" ht="33" customHeight="1">
+    <row r="8" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:4" ht="33" customHeight="1">
+    <row r="9" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="1:4" ht="22.9" customHeight="1">
+    <row r="10" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:4" ht="33" customHeight="1">
+    <row r="11" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:4" ht="22.9" customHeight="1">
+    <row r="12" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="11"/>
     </row>
-    <row r="13" spans="1:4" ht="33" customHeight="1">
+    <row r="13" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
     </row>
-    <row r="14" spans="1:4" ht="33" customHeight="1">
+    <row r="14" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:4" ht="22.9" customHeight="1">
+    <row r="15" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -717,17 +722,17 @@
       <c r="C15" s="7"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:4" ht="22.9" customHeight="1">
+    <row r="16" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
     </row>
-    <row r="17" ht="21" customHeight="1"/>
+    <row r="17" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="16">
     <mergeCell ref="B14:D14"/>

</xml_diff>